<commit_message>
reran yields w/ fluxes listed even if they're 0, to compare bounds
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP_kapps_only_for_rxns_used_in_kapp_calc/compiled_results.xlsx
+++ b/application/output_max_withoutMP_kapps_only_for_rxns_used_in_kapp_calc/compiled_results.xlsx
@@ -596,25 +596,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382212023962</v>
+        <v>17.81382211868636</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516930700739</v>
+        <v>0.5695516930204122</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>13.11829730685091</v>
+        <v>13.11830241409718</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4194242196246328</v>
+        <v>0.4194243829158536</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7364111541198238</v>
+        <v>0.7364114408853523</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -640,11 +640,11 @@
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>13.11829730685091</v>
+        <v>13.11830241409718</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
-        <v>0.4194242196246328</v>
+        <v>0.4194243829158536</v>
       </c>
     </row>
     <row r="3">
@@ -667,25 +667,25 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>2.555301936214222</v>
+        <v>2.555301938109797</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3122195089297514</v>
+        <v>0.3122195099690078</v>
       </c>
       <c r="G3" t="n">
-        <v>-5.549610217984472</v>
+        <v>-5.549610203628807</v>
       </c>
       <c r="H3" t="n">
-        <v>6.043377625746497</v>
+        <v>6.043377625746459</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3102110103118773</v>
+        <v>0.3102110103118753</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.993567030373089</v>
+        <v>0.9935670270658874</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -713,11 +713,11 @@
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>6.043377625746497</v>
+        <v>6.043377625746459</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
-        <v>0.3102110103118773</v>
+        <v>0.3102110103118753</v>
       </c>
     </row>
     <row r="4">
@@ -740,25 +740,25 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>7.379942361103544</v>
+        <v>7.379942361103503</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6654236103138855</v>
+        <v>0.6654236103138812</v>
       </c>
       <c r="G4" t="n">
-        <v>-5.545419566892341</v>
+        <v>-5.545419566892347</v>
       </c>
       <c r="H4" t="n">
-        <v>9.432019770030667</v>
+        <v>9.432019814940807</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3570109458354876</v>
+        <v>0.3570109475353793</v>
       </c>
       <c r="J4" t="n">
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5365167996775509</v>
+        <v>0.5365168022321551</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -786,11 +786,11 @@
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>9.432019770030667</v>
+        <v>9.432019814940807</v>
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="n">
-        <v>0.3570109458354876</v>
+        <v>0.3570109475353793</v>
       </c>
     </row>
     <row r="5">
@@ -813,25 +813,25 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>8.294245459149213</v>
+        <v>8.294245457651105</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7479521117530147</v>
+        <v>0.7479521116177738</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.544759808667549</v>
+        <v>-5.544759808668629</v>
       </c>
       <c r="H5" t="n">
-        <v>14.61087781511374</v>
+        <v>14.61087781511413</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5530356631391516</v>
+        <v>0.5530356631391665</v>
       </c>
       <c r="J5" t="n">
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7393998284769501</v>
+        <v>0.7393998286106646</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -859,11 +859,11 @@
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
-        <v>14.61087781511374</v>
+        <v>14.61087781511413</v>
       </c>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="n">
-        <v>0.5530356631391516</v>
+        <v>0.5530356631391665</v>
       </c>
     </row>
     <row r="6">
@@ -886,25 +886,25 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>7.379942361103544</v>
+        <v>7.379942361103503</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6654236103138855</v>
+        <v>0.6654236103138812</v>
       </c>
       <c r="G6" t="n">
-        <v>-5.545419566892341</v>
+        <v>-5.545419566892347</v>
       </c>
       <c r="H6" t="n">
-        <v>9.432019770030667</v>
+        <v>9.432019814940807</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3570109458354876</v>
+        <v>0.3570109475353793</v>
       </c>
       <c r="J6" t="n">
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5365167996775509</v>
+        <v>0.5365168022321551</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -932,11 +932,11 @@
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>9.432019770030667</v>
+        <v>9.432019814940807</v>
       </c>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="n">
-        <v>0.3570109458354876</v>
+        <v>0.3570109475353793</v>
       </c>
     </row>
     <row r="7">
@@ -959,25 +959,25 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>8.294245459149213</v>
+        <v>8.294245457651105</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7479521117530147</v>
+        <v>0.7479521116177738</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.544759808667549</v>
+        <v>-5.544759808668629</v>
       </c>
       <c r="H7" t="n">
-        <v>14.61087781511374</v>
+        <v>14.61087781511413</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5530356631391516</v>
+        <v>0.5530356631391665</v>
       </c>
       <c r="J7" t="n">
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7393998284769501</v>
+        <v>0.7393998286106646</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1005,11 +1005,11 @@
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
-        <v>14.61087781511374</v>
+        <v>14.61087781511413</v>
       </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="n">
-        <v>0.5530356631391516</v>
+        <v>0.5530356631391665</v>
       </c>
     </row>
     <row r="8">
@@ -1032,13 +1032,13 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>3.354728528907292</v>
+        <v>3.354728548864318</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4600748684385398</v>
+        <v>0.4600748711761332</v>
       </c>
       <c r="G8" t="n">
-        <v>-5.549441423005486</v>
+        <v>-5.549441422997732</v>
       </c>
       <c r="H8" t="n">
         <v>5.383403028843423</v>
@@ -1050,7 +1050,7 @@
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6741335888518062</v>
+        <v>0.6741335848404946</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1105,25 +1105,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697655376286</v>
+        <v>2.844697655376507</v>
       </c>
       <c r="F9" t="n">
-        <v>0.280099580945368</v>
+        <v>0.2800995809453898</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>1.412508608711654</v>
+        <v>1.412508608711675</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1390808856730769</v>
+        <v>0.139080885673079</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4965408559472423</v>
+        <v>0.496540855947211</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1149,11 +1149,11 @@
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>1.412508608711654</v>
+        <v>1.412508608711675</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
-        <v>0.1390808856730769</v>
+        <v>0.139080885673079</v>
       </c>
     </row>
     <row r="10">
@@ -1185,16 +1185,16 @@
         <v>-5.547686668594033</v>
       </c>
       <c r="H10" t="n">
-        <v>12.58150013552147</v>
+        <v>12.5815001355205</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4764332482263352</v>
+        <v>0.4764332482262986</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>1.054905917525079</v>
+        <v>1.054905917524998</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1222,11 +1222,11 @@
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>12.58150013552147</v>
+        <v>12.5815001355205</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
-        <v>0.4764332482263352</v>
+        <v>0.4764332482262986</v>
       </c>
     </row>
     <row r="11">
@@ -1249,25 +1249,25 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>4.161856556537502</v>
+        <v>4.161856555785772</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3085281699700423</v>
+        <v>0.3085281699143055</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.549820853803029</v>
+        <v>-5.549820853803196</v>
       </c>
       <c r="H11" t="n">
-        <v>9.577723638304525</v>
+        <v>9.577711144560674</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2982951305399613</v>
+        <v>0.2982947414263165</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.966832722499619</v>
+        <v>0.966831461481033</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1295,11 +1295,11 @@
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>9.577723638304525</v>
+        <v>9.577711144560674</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="n">
-        <v>0.2982951305399613</v>
+        <v>0.2982947414263165</v>
       </c>
     </row>
     <row r="12">
@@ -1331,16 +1331,16 @@
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>8.3262908855597</v>
+        <v>8.326290885559455</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5111522147960758</v>
+        <v>0.5111522147960607</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.6666701490697933</v>
+        <v>0.6666701490697735</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1366,11 +1366,11 @@
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>8.3262908855597</v>
+        <v>8.326290885559455</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
-        <v>0.5111522147960758</v>
+        <v>0.5111522147960607</v>
       </c>
     </row>
     <row r="13">
@@ -1393,25 +1393,25 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>2.611823947915461</v>
+        <v>2.611823932281909</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4262860847331228</v>
+        <v>0.4262860821805087</v>
       </c>
       <c r="G13" t="n">
-        <v>-5.548570274694224</v>
+        <v>-5.548570274707247</v>
       </c>
       <c r="H13" t="n">
-        <v>5.315708870631258</v>
+        <v>5.315708870631331</v>
       </c>
       <c r="I13" t="n">
-        <v>0.3644153964047416</v>
+        <v>0.3644153964047467</v>
       </c>
       <c r="J13" t="n">
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.854861111952281</v>
+        <v>0.8548611170712274</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1439,11 +1439,11 @@
       </c>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
-        <v>5.315708870631258</v>
+        <v>5.315708870631331</v>
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
-        <v>0.3644153964047416</v>
+        <v>0.3644153964047467</v>
       </c>
     </row>
     <row r="14">
@@ -1466,25 +1466,25 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>1.016994536421393</v>
+        <v>1.016994536421335</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2607839207207009</v>
+        <v>0.2607839207206863</v>
       </c>
       <c r="G14" t="n">
-        <v>-5.550180402242267</v>
+        <v>-5.550180402242266</v>
       </c>
       <c r="H14" t="n">
-        <v>1.322275094997493</v>
+        <v>1.322280786773293</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1424584749056315</v>
+        <v>0.1424590881227321</v>
       </c>
       <c r="J14" t="n">
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.5462701630987605</v>
+        <v>0.5462725145363295</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1512,11 +1512,11 @@
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
-        <v>1.322275094997493</v>
+        <v>1.322280786773293</v>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="n">
-        <v>0.1424584749056315</v>
+        <v>0.1424590881227321</v>
       </c>
     </row>
     <row r="15">
@@ -1539,25 +1539,25 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9874314721362993</v>
+        <v>0.9874314721362274</v>
       </c>
       <c r="F15" t="n">
-        <v>0.239394068030909</v>
+        <v>0.239394068030892</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.550717505065838</v>
+        <v>-5.55071750506583</v>
       </c>
       <c r="H15" t="n">
-        <v>1.344943131597913</v>
+        <v>1.344941371456769</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1370113824745772</v>
+        <v>0.1370112031663479</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.5723257205223948</v>
+        <v>0.5723249715137788</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1585,11 +1585,11 @@
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>1.344943131597913</v>
+        <v>1.344941371456769</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
-        <v>0.1370113824745772</v>
+        <v>0.1370112031663479</v>
       </c>
     </row>
     <row r="16">
@@ -1612,13 +1612,13 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>4.686403728372541</v>
+        <v>4.68640372837228</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3474539429141829</v>
+        <v>0.3474539429141642</v>
       </c>
       <c r="G16" t="n">
-        <v>-5.549184128068448</v>
+        <v>-5.549184128068436</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
@@ -1665,25 +1665,25 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>8.860211568548349</v>
+        <v>8.860211568542926</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7940334041382812</v>
+        <v>0.7940334041377936</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.51681017572383</v>
+        <v>-5.516810175723841</v>
       </c>
       <c r="H17" t="n">
-        <v>24.17540233688923</v>
+        <v>24.17540233686853</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9048021305862969</v>
+        <v>0.9048021305855222</v>
       </c>
       <c r="J17" t="n">
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>1.139501343231557</v>
+        <v>1.139501343231281</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1711,11 +1711,11 @@
       </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>24.17540233688923</v>
+        <v>24.17540233686853</v>
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
-        <v>0.9048021305862969</v>
+        <v>0.9048021305855222</v>
       </c>
     </row>
     <row r="18">
@@ -1738,25 +1738,25 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>3.836460769542236</v>
+        <v>3.83646076954262</v>
       </c>
       <c r="F18" t="n">
-        <v>0.537594161328863</v>
+        <v>0.5375941613289164</v>
       </c>
       <c r="G18" t="n">
-        <v>-5.5492542449107</v>
+        <v>-5.549254244910705</v>
       </c>
       <c r="H18" t="n">
-        <v>6.50500096918884</v>
+        <v>6.505000887552828</v>
       </c>
       <c r="I18" t="n">
-        <v>0.3829155054322021</v>
+        <v>0.3829155006267155</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7122761610462522</v>
+        <v>0.7122761521073072</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1784,11 +1784,11 @@
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>6.50500096918884</v>
+        <v>6.505000887552828</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
-        <v>0.3829155054322021</v>
+        <v>0.3829155006267155</v>
       </c>
     </row>
     <row r="19">
@@ -1820,16 +1820,16 @@
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>1.929450655511177</v>
+        <v>1.92945065551117</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2207242330273633</v>
+        <v>0.2207242330273625</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.4861187777464959</v>
+        <v>0.4861187777464941</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1855,11 +1855,11 @@
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>1.929450655511177</v>
+        <v>1.92945065551117</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="n">
-        <v>0.2207242330273633</v>
+        <v>0.2207242330273625</v>
       </c>
     </row>
     <row r="20">
@@ -1891,16 +1891,16 @@
         <v>-0.332925</v>
       </c>
       <c r="H20" t="n">
-        <v>0.097946072896019</v>
+        <v>0.097946031993648</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2307716612181017</v>
+        <v>0.2307715648476416</v>
       </c>
       <c r="J20" t="n">
         <v>-0.332925</v>
       </c>
       <c r="K20" t="n">
-        <v>0.9798169902750771</v>
+        <v>0.9798165811025918</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -1934,11 +1934,11 @@
       </c>
       <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="n">
-        <v>0.097946072896019</v>
+        <v>0.097946031993648</v>
       </c>
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="n">
-        <v>0.2307716612181017</v>
+        <v>0.2307715648476416</v>
       </c>
     </row>
     <row r="21">
@@ -1970,16 +1970,16 @@
         <v>-0.332925</v>
       </c>
       <c r="H21" t="n">
-        <v>0.111424668221153</v>
+        <v>0.111424668221111</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2370482663300356</v>
+        <v>0.2370482663299462</v>
       </c>
       <c r="J21" t="n">
         <v>-0.332925</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9759763714161513</v>
+        <v>0.9759763714157833</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2009,11 +2009,11 @@
       </c>
       <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="n">
-        <v>0.111424668221153</v>
+        <v>0.111424668221111</v>
       </c>
       <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="n">
-        <v>0.2370482663300356</v>
+        <v>0.2370482663299462</v>
       </c>
     </row>
     <row r="22">
@@ -2036,25 +2036,25 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>4.826633115573177</v>
+        <v>4.826633115573237</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4979383117364357</v>
+        <v>0.497938311736443</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.547262026771118</v>
+        <v>-5.547262026771105</v>
       </c>
       <c r="H22" t="n">
-        <v>8.258552528461752</v>
+        <v>8.258552528461658</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3577758749568217</v>
+        <v>0.3577758749568176</v>
       </c>
       <c r="J22" t="n">
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.7185144555540776</v>
+        <v>0.7185144555540589</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2082,11 +2082,11 @@
       </c>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
-        <v>8.258552528461752</v>
+        <v>8.258552528461658</v>
       </c>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="n">
-        <v>0.3577758749568217</v>
+        <v>0.3577758749568176</v>
       </c>
     </row>
     <row r="23">
@@ -2109,25 +2109,25 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143874209327</v>
+        <v>2.511143874209252</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710873793104</v>
+        <v>0.3475710873793001</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>1.166534631901427</v>
+        <v>1.166534079188301</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1614617603713631</v>
+        <v>0.1614616838695329</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.4645431286842252</v>
+        <v>0.4645429085801137</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2153,11 +2153,11 @@
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>1.166534631901427</v>
+        <v>1.166534079188301</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
-        <v>0.1614617603713631</v>
+        <v>0.1614616838695329</v>
       </c>
     </row>
     <row r="24">
@@ -2180,25 +2180,25 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>1.465955758988981</v>
+        <v>1.465955758988974</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3345898405304257</v>
+        <v>0.3345898405304245</v>
       </c>
       <c r="G24" t="n">
-        <v>-5.550743282537625</v>
+        <v>-5.550743282537618</v>
       </c>
       <c r="H24" t="n">
-        <v>1.929450655511192</v>
+        <v>1.929450655511212</v>
       </c>
       <c r="I24" t="n">
-        <v>0.1850435222999662</v>
+        <v>0.1850435222999681</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.5530458486325122</v>
+        <v>0.5530458486325199</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2226,11 +2226,11 @@
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>1.929450655511192</v>
+        <v>1.929450655511212</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
-        <v>0.1850435222999662</v>
+        <v>0.1850435222999681</v>
       </c>
     </row>
     <row r="25">
@@ -2262,16 +2262,16 @@
         <v>-5.550726324289684</v>
       </c>
       <c r="H25" t="n">
-        <v>1.397262464635824</v>
+        <v>1.397262464635801</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1446075126848192</v>
+        <v>0.1446075126848168</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.5260404297460085</v>
+        <v>0.5260404297459998</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2299,11 +2299,11 @@
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>1.397262464635824</v>
+        <v>1.397262464635801</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="n">
-        <v>0.1446075126848192</v>
+        <v>0.1446075126848168</v>
       </c>
     </row>
     <row r="26">
@@ -2326,25 +2326,25 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652187360732</v>
+        <v>9.725652187360838</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896739912092</v>
+        <v>0.7116896739912171</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>6.508474472797413</v>
+        <v>6.508474433991062</v>
       </c>
       <c r="I26" t="n">
-        <v>0.4762677079635825</v>
+        <v>0.4762677051238676</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.6692069948024361</v>
+        <v>0.6692069908123259</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2370,11 +2370,11 @@
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>6.508474472797413</v>
+        <v>6.508474433991062</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
-        <v>0.4762677079635825</v>
+        <v>0.4762677051238676</v>
       </c>
     </row>
     <row r="27">
@@ -2397,25 +2397,25 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013955884731691</v>
+        <v>0.1013955788142342</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406786063347258</v>
+        <v>0.2406785834077027</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
       </c>
       <c r="H27" t="n">
-        <v>0.099374624598613</v>
+        <v>0.099374631908636</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2358815261450911</v>
+        <v>0.2358815434965969</v>
       </c>
       <c r="J27" t="n">
         <v>-0.332925</v>
       </c>
       <c r="K27" t="n">
-        <v>0.9800685226548006</v>
+        <v>0.9800686881101517</v>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2445,11 +2445,11 @@
       </c>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="n">
-        <v>0.099374624598613</v>
+        <v>0.099374631908636</v>
       </c>
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="n">
-        <v>0.2358815261450911</v>
+        <v>0.2358815434965969</v>
       </c>
     </row>
     <row r="28">
@@ -2481,16 +2481,16 @@
         <v>-5.55073108000964</v>
       </c>
       <c r="H28" t="n">
-        <v>5.400062163986131</v>
+        <v>5.400062163986017</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2363232689206387</v>
+        <v>0.2363232689206337</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.9107025662341921</v>
+        <v>0.910702566234173</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2518,11 +2518,11 @@
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>5.400062163986131</v>
+        <v>5.400062163986017</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="n">
-        <v>0.2363232689206387</v>
+        <v>0.2363232689206337</v>
       </c>
     </row>
     <row r="29">
@@ -2554,16 +2554,16 @@
         <v>-2.20113372715757</v>
       </c>
       <c r="H29" t="n">
-        <v>0.125284854949458</v>
+        <v>0.125284854783982</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2604287968803942</v>
+        <v>0.2604287965364203</v>
       </c>
       <c r="J29" t="n">
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.9575253770609217</v>
+        <v>0.9575253757962239</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2595,11 +2595,11 @@
       </c>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
-        <v>0.125284854949458</v>
+        <v>0.125284854783982</v>
       </c>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
-        <v>0.2604287968803942</v>
+        <v>0.2604287965364203</v>
       </c>
     </row>
     <row r="30">
@@ -2622,10 +2622,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105612999394498</v>
+        <v>0.007105612030793992</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718414909479177</v>
+        <v>0.06718413993659518</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>

</xml_diff>

<commit_message>
minYield updated and fixed
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP_kapps_only_for_rxns_used_in_kapp_calc/compiled_results.xlsx
+++ b/application/output_max_withoutMP_kapps_only_for_rxns_used_in_kapp_calc/compiled_results.xlsx
@@ -596,10 +596,10 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.8138221557582</v>
+        <v>17.81382268889866</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516942056902</v>
+        <v>0.5695517112515016</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
@@ -614,7 +614,7 @@
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7364114393528272</v>
+        <v>0.7364114173131594</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -667,10 +667,10 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>6.941370064669262</v>
+        <v>6.941370272413776</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3563056214683741</v>
+        <v>0.3563056321320525</v>
       </c>
       <c r="G3" t="n">
         <v>-13.21</v>
@@ -685,7 +685,7 @@
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8706318161174728</v>
+        <v>0.8706317900608044</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -740,10 +740,10 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>20.06614449729091</v>
+        <v>20.06614509783982</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7595227110328777</v>
+        <v>0.759522733764227</v>
       </c>
       <c r="G4" t="n">
         <v>-13.21</v>
@@ -758,7 +758,7 @@
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4700464414683252</v>
+        <v>0.470046427400557</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -813,10 +813,10 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>22.34089329233793</v>
+        <v>22.34089326522185</v>
       </c>
       <c r="F5" t="n">
-        <v>0.845624122889358</v>
+        <v>0.8456241218629883</v>
       </c>
       <c r="G5" t="n">
         <v>-13.21</v>
@@ -831,7 +831,7 @@
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6539970279579241</v>
+        <v>0.653997028751708</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -886,10 +886,10 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>20.06614449729091</v>
+        <v>20.06614509783982</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7595227110328777</v>
+        <v>0.759522733764227</v>
       </c>
       <c r="G6" t="n">
         <v>-13.21</v>
@@ -904,7 +904,7 @@
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4700464414683252</v>
+        <v>0.470046427400557</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -959,10 +959,10 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.34089329233793</v>
+        <v>22.34089326522185</v>
       </c>
       <c r="F7" t="n">
-        <v>0.845624122889358</v>
+        <v>0.8456241218629883</v>
       </c>
       <c r="G7" t="n">
         <v>-13.21</v>
@@ -977,7 +977,7 @@
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.6539970279579241</v>
+        <v>0.653997028751708</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1032,10 +1032,10 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>9.055951952863756</v>
+        <v>9.055951957671432</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5217370667757679</v>
+        <v>0.5217370670527507</v>
       </c>
       <c r="G8" t="n">
         <v>-13.21</v>
@@ -1050,7 +1050,7 @@
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5944602021812885</v>
+        <v>0.594460201865698</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1105,10 +1105,10 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697658355452</v>
+        <v>2.844697753843605</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995812387078</v>
+        <v>0.2800995906408289</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
@@ -1123,7 +1123,7 @@
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4965408554272375</v>
+        <v>0.4965408387598184</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1176,10 +1176,10 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>12.89443785194213</v>
+        <v>12.89443799113937</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4882834990804356</v>
+        <v>0.4882835043515236</v>
       </c>
       <c r="G10" t="n">
         <v>-13.21</v>
@@ -1194,7 +1194,7 @@
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9757307980375048</v>
+        <v>0.9757307875043558</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1249,10 +1249,10 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>11.19787297467833</v>
+        <v>11.19787298372048</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3487541619380949</v>
+        <v>0.34875416221971</v>
       </c>
       <c r="G11" t="n">
         <v>-13.21</v>
@@ -1267,7 +1267,7 @@
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8553152162217491</v>
+        <v>0.8553152155310917</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1322,10 +1322,10 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880223</v>
+        <v>12.48937108880215</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293792</v>
+        <v>0.7667243171293745</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
@@ -1340,7 +1340,7 @@
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.6666701490697698</v>
+        <v>0.6666701490697738</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1393,10 +1393,10 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>7.096204240678009</v>
+        <v>7.096204247996516</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4864762432011431</v>
+        <v>0.4864762437028592</v>
       </c>
       <c r="G13" t="n">
         <v>-13.21</v>
@@ -1411,7 +1411,7 @@
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7490918652199673</v>
+        <v>0.7490918644474085</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1466,10 +1466,10 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>2.761960143974892</v>
+        <v>2.76196023337811</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2975663924620373</v>
+        <v>0.2975664020941072</v>
       </c>
       <c r="G14" t="n">
         <v>-13.21</v>
@@ -1484,7 +1484,7 @@
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.4787472366890582</v>
+        <v>0.4787472211922588</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1539,10 +1539,10 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>2.677177424089021</v>
+        <v>2.677177425269656</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2727280963681851</v>
+        <v>0.2727280964884582</v>
       </c>
       <c r="G15" t="n">
         <v>-13.21</v>
@@ -1557,7 +1557,7 @@
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.5023728944354221</v>
+        <v>0.5023728942138757</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1612,10 +1612,10 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>12.52385416926674</v>
+        <v>12.52385380260014</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3900514209184453</v>
+        <v>0.3900514094987314</v>
       </c>
       <c r="G16" t="n">
         <v>-13.21</v>
@@ -1665,10 +1665,10 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>24.24659203144867</v>
+        <v>24.24659199322306</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9074665159154658</v>
+        <v>0.907466514484813</v>
       </c>
       <c r="G17" t="n">
         <v>-13.21</v>
@@ -1683,7 +1683,7 @@
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>0.9970639298715548</v>
+        <v>0.9970639314434611</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1738,10 +1738,10 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>10.42241535579358</v>
+        <v>10.4224156636676</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6135132742779132</v>
+        <v>0.613513292400852</v>
       </c>
       <c r="G18" t="n">
         <v>-13.21</v>
@@ -1756,7 +1756,7 @@
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.6241356408749192</v>
+        <v>0.6241356224382005</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1811,10 +1811,10 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093041339537</v>
+        <v>3.969093169157485</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541189076495</v>
+        <v>0.4540541335296966</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
@@ -1829,7 +1829,7 @@
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.4861187771148835</v>
+        <v>0.4861187614602486</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1882,10 +1882,10 @@
         <v>268.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09996363129261256</v>
+        <v>0.09996363147194666</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2355252494837661</v>
+        <v>0.2355252499062969</v>
       </c>
       <c r="G20" t="n">
         <v>-0.332925</v>
@@ -1900,7 +1900,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K20" t="n">
-        <v>0.9798166665928864</v>
+        <v>0.9798166648351015</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -1961,10 +1961,10 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141673728959025</v>
+        <v>0.1141673732709542</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428831806141352</v>
+        <v>0.2428831814120316</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
@@ -1979,7 +1979,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9759764580263021</v>
+        <v>0.9759764548201183</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -2036,10 +2036,10 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>12.48937108880226</v>
+        <v>12.48937153880181</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5410628137990361</v>
+        <v>0.5410628332938546</v>
       </c>
       <c r="G22" t="n">
         <v>-13.21</v>
@@ -2054,7 +2054,7 @@
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.6612464686765634</v>
+        <v>0.6612464448514564</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2109,10 +2109,10 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143878215948</v>
+        <v>2.511143941130416</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710879338727</v>
+        <v>0.347571096641956</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
@@ -2127,7 +2127,7 @@
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.4645429078389048</v>
+        <v>0.4645428962001973</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2180,10 +2180,10 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>3.969093041339538</v>
+        <v>3.969093043938707</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3806549572065452</v>
+        <v>0.380654957455818</v>
       </c>
       <c r="G24" t="n">
         <v>-13.21</v>
@@ -2198,7 +2198,7 @@
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.4861187771148942</v>
+        <v>0.4861187767965582</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2253,10 +2253,10 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>2.957467104488082</v>
+        <v>2.957467102141706</v>
       </c>
       <c r="F25" t="n">
-        <v>0.306078473194127</v>
+        <v>0.3060784729512925</v>
       </c>
       <c r="G25" t="n">
         <v>-13.21</v>
@@ -2271,7 +2271,7 @@
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4724524112256044</v>
+        <v>0.4724524116004356</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2326,10 +2326,10 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652207600666</v>
+        <v>9.725652213171694</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896754722978</v>
+        <v>0.7116896758799663</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
@@ -2344,7 +2344,7 @@
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.669206989419655</v>
+        <v>0.6692069890363213</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2397,10 +2397,10 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013986989748657</v>
+        <v>0.1013955798081718</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406859896067657</v>
+        <v>0.2406785857669721</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
@@ -2415,7 +2415,7 @@
         <v>-0.332925</v>
       </c>
       <c r="K27" t="n">
-        <v>0.9800385302110093</v>
+        <v>0.9800686785029569</v>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -2472,10 +2472,10 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>6.766253892867912</v>
+        <v>6.766253899865699</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2961120057049863</v>
+        <v>0.2961120060112309</v>
       </c>
       <c r="G28" t="n">
         <v>-13.21</v>
@@ -2490,7 +2490,7 @@
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.7980874276204809</v>
+        <v>0.7980874267950838</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2545,10 +2545,10 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423263314998</v>
+        <v>0.1308423266048828</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810757756068</v>
+        <v>0.2719810763438862</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
@@ -2563,7 +2563,7 @@
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.9575254300092648</v>
+        <v>0.9575254280086036</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2622,10 +2622,10 @@
         <v>126.11004</v>
       </c>
       <c r="E30" t="n">
-        <v>0.007105612876140991</v>
+        <v>0.00710589806189561</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06718414792941983</v>
+        <v>0.06718684438393539</v>
       </c>
       <c r="G30" t="n">
         <v>-0.078476895921783</v>

</xml_diff>